<commit_message>
Result to test 100
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescoverolla/Desktop/UNI/ASSSC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D7ACA35-3044-EB4C-BA60-98BBCB99C310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70832BB9-7F41-C64A-BC3B-E37252989609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18120" yWindow="6820" windowWidth="28040" windowHeight="17440" xr2:uid="{8173C7AF-BEEB-1146-8A2D-8A9248A9A970}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,6 +537,9 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C5">
+        <v>48.489703333333303</v>
+      </c>
     </row>
     <row r="6" spans="1:25" ht="26" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -616,6 +619,9 @@
     <row r="9" spans="1:25" ht="26" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="C9">
+        <v>309.050223783506</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>